<commit_message>
updated for city search and missing city list
</commit_message>
<xml_diff>
--- a/read me.xlsx
+++ b/read me.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="Data validation" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>SQL Queries</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Random test screen print is as below:</t>
+  </si>
+  <si>
+    <t>CZECH REPUBLIC</t>
   </si>
 </sst>
 </file>
@@ -195,19 +198,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>75334</xdr:rowOff>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -220,8 +223,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1" y="5905500"/>
-          <a:ext cx="10153649" cy="6933334"/>
+          <a:off x="0" y="952499"/>
+          <a:ext cx="10382249" cy="5324475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -234,18 +237,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>456808</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9067801</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="12" name="Picture 11"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -258,8 +261,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1" y="13144500"/>
-          <a:ext cx="10848582" cy="5781675"/>
+          <a:off x="1" y="6667500"/>
+          <a:ext cx="9067800" cy="5915025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>176164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="13906500"/>
+          <a:ext cx="10696575" cy="5700664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -277,27 +318,103 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>75334</xdr:rowOff>
+      <xdr:colOff>456808</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="15" name="Picture 14"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1" y="19240500"/>
-          <a:ext cx="10601324" cy="6933334"/>
+          <a:off x="1" y="20002500"/>
+          <a:ext cx="10848582" cy="6334125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="27051000"/>
+          <a:ext cx="11572874" cy="5400675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="32956499"/>
+          <a:ext cx="11391900" cy="6791325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -310,32 +427,32 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>16121</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="18" name="Picture 17"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="26670000"/>
-          <a:ext cx="10620375" cy="5543550"/>
+          <a:off x="0" y="40195500"/>
+          <a:ext cx="10753725" cy="5731121"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -348,132 +465,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>176</xdr:row>
+      <xdr:row>242</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>179350</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>75334</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>145706</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="32766000"/>
-          <a:ext cx="13009525" cy="6933334"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>214</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>243</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="40005000"/>
-          <a:ext cx="9972675" cy="5572125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>245</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>179350</xdr:colOff>
-      <xdr:row>281</xdr:row>
-      <xdr:rowOff>75334</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="45910500"/>
-          <a:ext cx="13009525" cy="6933334"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>283</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>179350</xdr:colOff>
-      <xdr:row>319</xdr:row>
-      <xdr:rowOff>75334</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPr id="19" name="Picture 18"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -486,8 +489,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="53149500"/>
-          <a:ext cx="13009525" cy="6933334"/>
+          <a:off x="0" y="46101000"/>
+          <a:ext cx="10639425" cy="5670206"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -500,18 +503,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>87468</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPr id="21" name="Picture 20"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -524,8 +527,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1" y="1143000"/>
-          <a:ext cx="10172700" cy="5421468"/>
+          <a:off x="1" y="52387499"/>
+          <a:ext cx="10439400" cy="6448425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>153181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="59626500"/>
+          <a:ext cx="11010900" cy="5868181"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -824,9 +865,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A283"/>
+  <dimension ref="A1:A313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="D304" sqref="D304"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -873,29 +916,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="6" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="6" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="6" t="s">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="6" t="s">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>